<commit_message>
Last Update after Second Evaluation
</commit_message>
<xml_diff>
--- a/Descriptor_Objetos.xlsx
+++ b/Descriptor_Objetos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t xml:space="preserve">TR_ID_CIUDAD </t>
   </si>
@@ -861,13 +861,67 @@
       </rPr>
       <t xml:space="preserve"> ( pID_PARTIDO RESULTADO.ID_PARTIDO%TYPE, pPRIMERT_GOLES_EQUIPO1 RESULTADO.PRIMERT_GOLES_EQUIPO1%TYPE, pPRIMERT_GOLES_EQUIPO2 RESULTADO.PRIMERT_GOLES_EQUIPO2%TYPE, pSEGUNDOT_GOLES_EQUIPO1 RESULTADO.SEGUNDOT_GOLES_EQUIPO1%TYPE, pSEGUNDOT_GOLES_EQUIPO2 RESULTADO.SEGUNDOT_GOLES_EQUIPO2%TYPE, pTIEMPOEXTRA_GOLES_EQUIPO1 RESULTADO.TIEMPOEXTRA_GOLES_EQUIPO1%TYPE, pTIEMPOEXTRA_GOLES_EQUIPO2 RESULTADO.TIEMPOEXTRA_GOLES_EQUIPO2%TYPE, pPENALES_GOLES_EQUIPO1 RESULTADO.PENALES_GOLES_EQUIPO1%TYPE, pPENALES_GOLES_EQUIPO2 RESULTADO.PENALES_GOLES_EQUIPO2%TYPE, pTARJETAS_A_EQUIPO1 RESULTADO.TARJETAS_A_EQUIPO1%TYPE, pTARJETAS_A_EQUIPO2 RESULTADO.TARJETAS_A_EQUIPO2%TYPE, pTARJETAS_R_EQUIPO1 RESULTADO.TARJETAS_R_EQUIPO1%TYPE, pTARJETAS_R_EQUIPO2 RESULTADO.TARJETAS_R_EQUIPO2%TYPE, pID_RESULTADO RESULTADO.ID_RESULTADO%TYPE)</t>
     </r>
+  </si>
+  <si>
+    <t>FN_PARTIDO_COMPETENCIAS_SELECT(INTEGER)</t>
+  </si>
+  <si>
+    <t>FN_PARTIDO_ALLCOMPETE_SELECT</t>
+  </si>
+  <si>
+    <t>FN_GET_EQUIPOS_COMPETENCIAS(INTEGER)</t>
+  </si>
+  <si>
+    <t>FN_GETALL_EQUIPOS_COMPETENCIAS</t>
+  </si>
+  <si>
+    <t>FN_COMP_RESULTADO_SELECT(INTEGER)</t>
+  </si>
+  <si>
+    <t>TRIGGER QUE INSERTA UN VALOR AUTONUMERICO DE CADA CAMPO ID DE CADA TABLA</t>
+  </si>
+  <si>
+    <t>FUNCIONES QUE RETORNAN LA INFORMACION DE LA TABLAS DE ACUERDO AL FILTRO (PARAMETRO)</t>
+  </si>
+  <si>
+    <t>FUNCION PARA OBTENER EL NOMBRE DE UN EQUIPO</t>
+  </si>
+  <si>
+    <t>FUNCIONES QUE RETORNAN EL PRIMER REPORTE</t>
+  </si>
+  <si>
+    <t>FUNCIONES QUE RETORNAN EL SEGUNDO REPORTE</t>
+  </si>
+  <si>
+    <t>FUNCION QUE RETORNA EL TERCER REPORTE</t>
+  </si>
+  <si>
+    <t>PROCEDIMIENOS ALMACENADOS PARA LA INSERCION DE DATOS A CADA TABLA</t>
+  </si>
+  <si>
+    <t>PROCEDIMIENTOS ALMACENADOS PARA ELIMINAR DATOS DE CADA UNA DE LAS TABLAS</t>
+  </si>
+  <si>
+    <t>PROCEDIMIENOS ALMACENADOS PARA LA ACTUALIZACION DE LOS DATOS DE CADA UNA DE LAS TABLAS</t>
+  </si>
+  <si>
+    <t>INFORME DESCRIPTIVO DE LOS OBJETOS DE LA BASE DE DATOS</t>
+  </si>
+  <si>
+    <t>PROYECTO TEORIA BASE DE DATOS 1</t>
+  </si>
+  <si>
+    <t>COMPETENCIAS DE FUTBOL</t>
+  </si>
+  <si>
+    <t>POR: CRISTIAN PAVEL LARA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -883,8 +937,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -897,8 +974,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -906,26 +989,154 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1207,7 +1418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C68"/>
+  <dimension ref="B2:C76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1220,350 +1431,484 @@
     <col min="3" max="3" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B3" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="C18" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="11"/>
+    </row>
+    <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="13"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="13"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="C36" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="C37" s="10"/>
+    </row>
+    <row r="38" spans="2:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="2:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="2:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+      <c r="C42" s="10"/>
+    </row>
+    <row r="43" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="C43" s="10"/>
+    </row>
+    <row r="44" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="2:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+      <c r="C45" s="10"/>
+    </row>
+    <row r="46" spans="2:3" ht="360" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+      <c r="C46" s="10"/>
+    </row>
+    <row r="47" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+      <c r="C47" s="10"/>
+    </row>
+    <row r="48" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="2:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+      <c r="C48" s="10"/>
+    </row>
+    <row r="49" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="2:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+      <c r="C49" s="10"/>
+    </row>
+    <row r="50" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+      <c r="C50" s="11"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+      <c r="C51" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+      <c r="C52" s="10"/>
+    </row>
+    <row r="53" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+      <c r="C54" s="10"/>
+    </row>
+    <row r="55" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="C55" s="10"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+      <c r="C56" s="10"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+      <c r="C57" s="10"/>
+    </row>
+    <row r="58" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+      <c r="C58" s="10"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+      <c r="C59" s="10"/>
+    </row>
+    <row r="60" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+      <c r="C60" s="10"/>
+    </row>
+    <row r="61" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+      <c r="C61" s="10"/>
+    </row>
+    <row r="62" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+      <c r="C62" s="10"/>
+    </row>
+    <row r="63" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+      <c r="C63" s="10"/>
+    </row>
+    <row r="64" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+      <c r="C64" s="10"/>
+    </row>
+    <row r="65" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="C65" s="11"/>
+    </row>
+    <row r="66" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+      <c r="C66" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="2:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+      <c r="C67" s="10"/>
+    </row>
+    <row r="68" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="2:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+      <c r="C68" s="10"/>
+    </row>
+    <row r="69" spans="2:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="2:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+      <c r="C69" s="10"/>
+    </row>
+    <row r="70" spans="2:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="B70" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="2:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+      <c r="C70" s="10"/>
+    </row>
+    <row r="71" spans="2:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="2:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+      <c r="C71" s="10"/>
+    </row>
+    <row r="72" spans="2:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B72" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+      <c r="C72" s="10"/>
+    </row>
+    <row r="73" spans="2:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B73" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+      <c r="C73" s="10"/>
+    </row>
+    <row r="74" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="2:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+      <c r="C74" s="10"/>
+    </row>
+    <row r="75" spans="2:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="2:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+      <c r="C75" s="10"/>
+    </row>
+    <row r="76" spans="2:3" ht="360" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="C76" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B26:C26"/>
+  <mergeCells count="10">
+    <mergeCell ref="C36:C50"/>
+    <mergeCell ref="C51:C65"/>
+    <mergeCell ref="C66:C76"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="C8:C16"/>
+    <mergeCell ref="C18:C28"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>